<commit_message>
Added Hydrogen OCGT to TYNDP-2024_National_Trends.xlsx unittypedata
</commit_message>
<xml_diff>
--- a/src_files/data_files/TYNDP-2024_National_Trends.xlsx
+++ b/src_files/data_files/TYNDP-2024_National_Trends.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ehjeric\git_backbone\balticseah2\backbone_250414\north_european_model_tyndp2024_update\src_files\data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9609AAF9-6F94-427C-958C-7F662B8CA317}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F42ACA6-5046-456A-A429-9D5B92FC956F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="9" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2736" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2744" uniqueCount="270">
   <si>
     <t>Country</t>
   </si>
@@ -840,32 +840,6 @@
   </si>
   <si>
     <t>Manually added sheets</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>unittypedata</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, with parameters for Hydrogen CCGT.</t>
-    </r>
   </si>
   <si>
     <r>
@@ -1019,6 +993,38 @@
     <t xml:space="preserve">
 Column(s)</t>
   </si>
+  <si>
+    <t>Hydrogen OCGT</t>
+  </si>
+  <si>
+    <t>hydrogenOCGT</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>unittypedata</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, with parameters for Hydrogen CCGT and Hydrogen OCGT.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -1027,7 +1033,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1039,6 +1045,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1114,6 +1121,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="13">
@@ -1247,7 +1265,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1360,6 +1378,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -2137,8 +2163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AC769E0-33E8-4D95-B061-5C4E37A4649E}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2156,10 +2182,10 @@
         <v>146</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="75">
@@ -2167,7 +2193,7 @@
         <v>147</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="14"/>
@@ -2177,7 +2203,7 @@
     <row r="4" spans="1:6" ht="30.75" customHeight="1">
       <c r="A4" s="14"/>
       <c r="B4" s="20" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C4" s="21" t="s">
         <v>145</v>
@@ -2204,7 +2230,7 @@
         <v>142</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
@@ -2216,7 +2242,7 @@
         <v>200</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
@@ -2228,7 +2254,7 @@
         <v>141</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
@@ -2240,7 +2266,7 @@
         <v>140</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
@@ -2252,7 +2278,7 @@
         <v>139</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
@@ -2405,17 +2431,17 @@
         <v>255</v>
       </c>
       <c r="B25" t="s">
-        <v>256</v>
+        <v>269</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="B26" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="B27" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -3639,8 +3665,8 @@
   </sheetPr>
   <dimension ref="A1:H548"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E548" sqref="E2:E548"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12999,7 +13025,7 @@
   </sheetPr>
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2:F41"/>
     </sheetView>
   </sheetViews>
@@ -16651,10 +16677,10 @@
   <sheetPr>
     <tabColor theme="6" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:AP2"/>
+  <dimension ref="A1:AP3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="AN6" sqref="AN6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16832,7 +16858,7 @@
         <v>2</v>
       </c>
       <c r="W2">
-        <v>4.0999999999999996</v>
+        <v>7.6</v>
       </c>
       <c r="X2">
         <v>25.06</v>
@@ -16871,15 +16897,113 @@
         <v>198</v>
       </c>
       <c r="AP2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="3" spans="1:42">
+      <c r="A3" s="41" t="s">
+        <v>189</v>
+      </c>
+      <c r="B3" s="44">
+        <v>1</v>
+      </c>
+      <c r="C3" s="42" t="s">
+        <v>267</v>
+      </c>
+      <c r="D3" s="43" t="s">
+        <v>268</v>
+      </c>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42" t="s">
+        <v>191</v>
+      </c>
+      <c r="K3" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="42"/>
+      <c r="O3" s="42">
+        <v>0.42</v>
+      </c>
+      <c r="P3" s="42">
+        <v>0.42</v>
+      </c>
+      <c r="Q3" s="42">
+        <v>0.4</v>
+      </c>
+      <c r="R3" s="43">
+        <v>1</v>
+      </c>
+      <c r="S3" s="42">
+        <v>1.6</v>
+      </c>
+      <c r="T3" s="42"/>
+      <c r="U3" s="42">
+        <v>1</v>
+      </c>
+      <c r="V3" s="42">
+        <v>1</v>
+      </c>
+      <c r="W3" s="42">
+        <v>0.21</v>
+      </c>
+      <c r="X3" s="42">
+        <v>20.36</v>
+      </c>
+      <c r="Y3" s="42">
+        <v>0.25</v>
+      </c>
+      <c r="Z3" s="42">
+        <v>24.28</v>
+      </c>
+      <c r="AA3" s="42">
+        <v>0.2</v>
+      </c>
+      <c r="AB3" s="42">
+        <v>17.23</v>
+      </c>
+      <c r="AC3" s="42">
+        <v>2</v>
+      </c>
+      <c r="AD3" s="42">
+        <v>3</v>
+      </c>
+      <c r="AE3" s="42">
+        <v>0.12</v>
+      </c>
+      <c r="AF3" s="42">
+        <v>0.12</v>
+      </c>
+      <c r="AG3" s="42"/>
+      <c r="AH3" s="42"/>
+      <c r="AI3" s="42"/>
+      <c r="AJ3" s="42">
+        <v>24.28</v>
+      </c>
+      <c r="AK3" s="42"/>
+      <c r="AL3" s="42"/>
+      <c r="AN3" t="s">
+        <v>244</v>
+      </c>
+      <c r="AO3" s="36" t="s">
+        <v>198</v>
+      </c>
+      <c r="AP3" t="s">
         <v>243</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="AO2" r:id="rId1" display="https://www.entsoe.eu/eraa/2024/downloads/" xr:uid="{67CF8E31-412D-4600-8E5C-38B0E7B92D2F}"/>
+    <hyperlink ref="AO3" r:id="rId2" display="https://www.entsoe.eu/eraa/2024/downloads/" xr:uid="{334C4004-95A7-4DDB-8754-28228847097F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added missing NOS0-UK00 transmission line to transferdata
</commit_message>
<xml_diff>
--- a/src_files/data_files/TYNDP-2024_National_Trends.xlsx
+++ b/src_files/data_files/TYNDP-2024_National_Trends.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BB\bb-master\north_european_model\src_files\data_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ehjeric\git_backbone\balticseah2\backbone_250414\north_european_model\src_files\data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA0696F-3EBF-4E06-9F17-9DA1D07A7E25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53FF571A-DBF3-41B8-86D0-5D9E3BDCD9AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="862" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="862" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="9" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2958" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2968" uniqueCount="259">
   <si>
     <t>Country</t>
   </si>
@@ -987,6 +987,9 @@
   </si>
   <si>
     <t>Constant_share</t>
+  </si>
+  <si>
+    <t>NOS0-UK00</t>
   </si>
 </sst>
 </file>
@@ -1781,8 +1784,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{B440C99F-3BB1-4A8C-9867-FC60A58307DE}" name="Table6" displayName="Table6" ref="A1:K91" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8">
-  <autoFilter ref="A1:K91" xr:uid="{B440C99F-3BB1-4A8C-9867-FC60A58307DE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{B440C99F-3BB1-4A8C-9867-FC60A58307DE}" name="Table6" displayName="Table6" ref="A1:K93" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8">
+  <autoFilter ref="A1:K93" xr:uid="{B440C99F-3BB1-4A8C-9867-FC60A58307DE}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{02926FC6-CA21-44BB-975F-A929C6C412D4}" name="from-to"/>
     <tableColumn id="2" xr3:uid="{9A1A3B49-8442-4D63-8194-9CB505844700}" name="from"/>
@@ -3096,7 +3099,7 @@
   </sheetPr>
   <dimension ref="A1:H616"/>
   <sheetViews>
-    <sheetView topLeftCell="A310" workbookViewId="0">
+    <sheetView topLeftCell="A110" workbookViewId="0">
       <selection activeCell="M380" sqref="M380"/>
     </sheetView>
   </sheetViews>
@@ -14406,10 +14409,10 @@
   <sheetPr>
     <tabColor theme="6" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:K91"/>
+  <dimension ref="A1:K93"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A89" sqref="A89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15886,13 +15889,13 @@
     </row>
     <row r="43" spans="1:11">
       <c r="A43" t="s">
-        <v>131</v>
+        <v>258</v>
       </c>
       <c r="B43" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C43" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D43" t="s">
         <v>7</v>
@@ -15904,13 +15907,13 @@
         <v>2030</v>
       </c>
       <c r="G43">
-        <v>600</v>
+        <v>1400</v>
       </c>
       <c r="H43">
-        <v>600</v>
+        <v>1400</v>
       </c>
       <c r="I43">
-        <v>8.3330000000000001E-3</v>
+        <v>2.7680000000000001E-3</v>
       </c>
       <c r="J43">
         <v>1</v>
@@ -15921,13 +15924,13 @@
     </row>
     <row r="44" spans="1:11">
       <c r="A44" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B44" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C44" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D44" t="s">
         <v>7</v>
@@ -15939,13 +15942,13 @@
         <v>2030</v>
       </c>
       <c r="G44">
-        <v>3300</v>
+        <v>600</v>
       </c>
       <c r="H44">
-        <v>3300</v>
+        <v>600</v>
       </c>
       <c r="I44">
-        <v>2.1359999999999999E-3</v>
+        <v>8.3330000000000001E-3</v>
       </c>
       <c r="J44">
         <v>1</v>
@@ -15956,13 +15959,13 @@
     </row>
     <row r="45" spans="1:11">
       <c r="A45" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B45" t="s">
+        <v>23</v>
+      </c>
+      <c r="C45" t="s">
         <v>24</v>
-      </c>
-      <c r="C45" t="s">
-        <v>25</v>
       </c>
       <c r="D45" t="s">
         <v>7</v>
@@ -15974,13 +15977,13 @@
         <v>2030</v>
       </c>
       <c r="G45">
-        <v>7300</v>
+        <v>3300</v>
       </c>
       <c r="H45">
-        <v>7300</v>
+        <v>3300</v>
       </c>
       <c r="I45">
-        <v>1.8680000000000001E-3</v>
+        <v>2.1359999999999999E-3</v>
       </c>
       <c r="J45">
         <v>1</v>
@@ -15991,13 +15994,13 @@
     </row>
     <row r="46" spans="1:11">
       <c r="A46" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B46" t="s">
+        <v>24</v>
+      </c>
+      <c r="C46" t="s">
         <v>25</v>
-      </c>
-      <c r="C46" t="s">
-        <v>26</v>
       </c>
       <c r="D46" t="s">
         <v>7</v>
@@ -16009,13 +16012,13 @@
         <v>2030</v>
       </c>
       <c r="G46">
-        <v>6200</v>
+        <v>7300</v>
       </c>
       <c r="H46">
-        <v>2800</v>
+        <v>7300</v>
       </c>
       <c r="I46">
-        <v>2.679E-3</v>
+        <v>1.8680000000000001E-3</v>
       </c>
       <c r="J46">
         <v>1</v>
@@ -16026,13 +16029,13 @@
     </row>
     <row r="47" spans="1:11">
       <c r="A47" t="s">
-        <v>247</v>
+        <v>134</v>
       </c>
       <c r="B47" t="s">
-        <v>245</v>
+        <v>25</v>
       </c>
       <c r="C47" t="s">
-        <v>246</v>
+        <v>26</v>
       </c>
       <c r="D47" t="s">
         <v>7</v>
@@ -16041,16 +16044,16 @@
         <v>8</v>
       </c>
       <c r="F47">
-        <v>2040</v>
+        <v>2030</v>
       </c>
       <c r="G47">
-        <v>1200</v>
+        <v>6200</v>
       </c>
       <c r="H47">
-        <v>1200</v>
+        <v>2800</v>
       </c>
       <c r="I47">
-        <v>8.7790000000000003E-3</v>
+        <v>2.679E-3</v>
       </c>
       <c r="J47">
         <v>1</v>
@@ -16061,13 +16064,13 @@
     </row>
     <row r="48" spans="1:11">
       <c r="A48" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B48" t="s">
         <v>245</v>
       </c>
       <c r="C48" t="s">
-        <v>9</v>
+        <v>246</v>
       </c>
       <c r="D48" t="s">
         <v>7</v>
@@ -16079,13 +16082,13 @@
         <v>2040</v>
       </c>
       <c r="G48">
-        <v>7500</v>
+        <v>1200</v>
       </c>
       <c r="H48">
-        <v>7500</v>
+        <v>1200</v>
       </c>
       <c r="I48">
-        <v>2.134E-3</v>
+        <v>8.7790000000000003E-3</v>
       </c>
       <c r="J48">
         <v>1</v>
@@ -16096,10 +16099,10 @@
     </row>
     <row r="49" spans="1:11">
       <c r="A49" t="s">
-        <v>94</v>
+        <v>248</v>
       </c>
       <c r="B49" t="s">
-        <v>6</v>
+        <v>245</v>
       </c>
       <c r="C49" t="s">
         <v>9</v>
@@ -16114,13 +16117,13 @@
         <v>2040</v>
       </c>
       <c r="G49">
-        <v>1000</v>
+        <v>7500</v>
       </c>
       <c r="H49">
-        <v>1000</v>
+        <v>7500</v>
       </c>
       <c r="I49">
-        <v>9.5930000000000008E-3</v>
+        <v>2.134E-3</v>
       </c>
       <c r="J49">
         <v>1</v>
@@ -16131,13 +16134,13 @@
     </row>
     <row r="50" spans="1:11">
       <c r="A50" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B50" t="s">
         <v>6</v>
       </c>
       <c r="C50" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D50" t="s">
         <v>7</v>
@@ -16149,13 +16152,13 @@
         <v>2040</v>
       </c>
       <c r="G50">
-        <v>3800</v>
+        <v>1000</v>
       </c>
       <c r="H50">
-        <v>5300</v>
+        <v>1000</v>
       </c>
       <c r="I50">
-        <v>4.0200000000000001E-3</v>
+        <v>9.5930000000000008E-3</v>
       </c>
       <c r="J50">
         <v>1</v>
@@ -16166,13 +16169,13 @@
     </row>
     <row r="51" spans="1:11">
       <c r="A51" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B51" t="s">
         <v>6</v>
       </c>
       <c r="C51" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D51" t="s">
         <v>7</v>
@@ -16184,13 +16187,13 @@
         <v>2040</v>
       </c>
       <c r="G51">
-        <v>5400</v>
+        <v>3800</v>
       </c>
       <c r="H51">
-        <v>4400</v>
+        <v>5300</v>
       </c>
       <c r="I51">
-        <v>4.6319999999999998E-3</v>
+        <v>4.0200000000000001E-3</v>
       </c>
       <c r="J51">
         <v>1</v>
@@ -16201,13 +16204,13 @@
     </row>
     <row r="52" spans="1:11">
       <c r="A52" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B52" t="s">
         <v>6</v>
       </c>
       <c r="C52" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D52" t="s">
         <v>7</v>
@@ -16219,13 +16222,13 @@
         <v>2040</v>
       </c>
       <c r="G52">
-        <v>4800</v>
+        <v>5400</v>
       </c>
       <c r="H52">
-        <v>4800</v>
+        <v>4400</v>
       </c>
       <c r="I52">
-        <v>8.4419999999999999E-3</v>
+        <v>4.6319999999999998E-3</v>
       </c>
       <c r="J52">
         <v>1</v>
@@ -16236,13 +16239,13 @@
     </row>
     <row r="53" spans="1:11">
       <c r="A53" t="s">
-        <v>249</v>
+        <v>97</v>
       </c>
       <c r="B53" t="s">
-        <v>246</v>
+        <v>6</v>
       </c>
       <c r="C53" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="D53" t="s">
         <v>7</v>
@@ -16254,13 +16257,13 @@
         <v>2040</v>
       </c>
       <c r="G53">
-        <v>4500</v>
+        <v>4800</v>
       </c>
       <c r="H53">
-        <v>5000</v>
+        <v>4800</v>
       </c>
       <c r="I53">
-        <v>5.7710000000000001E-3</v>
+        <v>8.4419999999999999E-3</v>
       </c>
       <c r="J53">
         <v>1</v>
@@ -16271,13 +16274,13 @@
     </row>
     <row r="54" spans="1:11">
       <c r="A54" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B54" t="s">
         <v>246</v>
       </c>
       <c r="C54" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D54" t="s">
         <v>7</v>
@@ -16289,13 +16292,13 @@
         <v>2040</v>
       </c>
       <c r="G54">
-        <v>2200</v>
+        <v>4500</v>
       </c>
       <c r="H54">
-        <v>4500</v>
+        <v>5000</v>
       </c>
       <c r="I54">
-        <v>7.3699999999999998E-3</v>
+        <v>5.7710000000000001E-3</v>
       </c>
       <c r="J54">
         <v>1</v>
@@ -16306,13 +16309,13 @@
     </row>
     <row r="55" spans="1:11">
       <c r="A55" t="s">
-        <v>98</v>
+        <v>250</v>
       </c>
       <c r="B55" t="s">
-        <v>9</v>
+        <v>246</v>
       </c>
       <c r="C55" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D55" t="s">
         <v>7</v>
@@ -16327,10 +16330,10 @@
         <v>2200</v>
       </c>
       <c r="H55">
-        <v>3000</v>
+        <v>4500</v>
       </c>
       <c r="I55">
-        <v>5.143E-3</v>
+        <v>7.3699999999999998E-3</v>
       </c>
       <c r="J55">
         <v>1</v>
@@ -16341,13 +16344,13 @@
     </row>
     <row r="56" spans="1:11">
       <c r="A56" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B56" t="s">
         <v>9</v>
       </c>
       <c r="C56" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D56" t="s">
         <v>7</v>
@@ -16359,13 +16362,13 @@
         <v>2040</v>
       </c>
       <c r="G56">
-        <v>3500</v>
+        <v>2200</v>
       </c>
       <c r="H56">
-        <v>3500</v>
+        <v>3000</v>
       </c>
       <c r="I56">
-        <v>4.2859999999999999E-3</v>
+        <v>5.143E-3</v>
       </c>
       <c r="J56">
         <v>1</v>
@@ -16376,13 +16379,13 @@
     </row>
     <row r="57" spans="1:11">
       <c r="A57" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B57" t="s">
         <v>9</v>
       </c>
       <c r="C57" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D57" t="s">
         <v>7</v>
@@ -16394,13 +16397,13 @@
         <v>2040</v>
       </c>
       <c r="G57">
-        <v>4800</v>
+        <v>3500</v>
       </c>
       <c r="H57">
-        <v>4800</v>
+        <v>3500</v>
       </c>
       <c r="I57">
-        <v>4.2189999999999997E-3</v>
+        <v>4.2859999999999999E-3</v>
       </c>
       <c r="J57">
         <v>1</v>
@@ -16411,13 +16414,13 @@
     </row>
     <row r="58" spans="1:11">
       <c r="A58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B58" t="s">
         <v>9</v>
       </c>
       <c r="C58" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D58" t="s">
         <v>7</v>
@@ -16429,13 +16432,13 @@
         <v>2040</v>
       </c>
       <c r="G58">
-        <v>5000</v>
+        <v>4800</v>
       </c>
       <c r="H58">
-        <v>5000</v>
+        <v>4800</v>
       </c>
       <c r="I58">
-        <v>2.7590000000000002E-3</v>
+        <v>4.2189999999999997E-3</v>
       </c>
       <c r="J58">
         <v>1</v>
@@ -16446,13 +16449,13 @@
     </row>
     <row r="59" spans="1:11">
       <c r="A59" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B59" t="s">
         <v>9</v>
       </c>
       <c r="C59" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D59" t="s">
         <v>7</v>
@@ -16464,13 +16467,13 @@
         <v>2040</v>
       </c>
       <c r="G59">
-        <v>1400</v>
+        <v>5000</v>
       </c>
       <c r="H59">
-        <v>1400</v>
+        <v>5000</v>
       </c>
       <c r="I59">
-        <v>3.571E-3</v>
+        <v>2.7590000000000002E-3</v>
       </c>
       <c r="J59">
         <v>1</v>
@@ -16481,13 +16484,13 @@
     </row>
     <row r="60" spans="1:11">
       <c r="A60" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B60" t="s">
         <v>9</v>
       </c>
       <c r="C60" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D60" t="s">
         <v>7</v>
@@ -16499,13 +16502,13 @@
         <v>2040</v>
       </c>
       <c r="G60">
-        <v>2000</v>
+        <v>1400</v>
       </c>
       <c r="H60">
-        <v>3000</v>
+        <v>1400</v>
       </c>
       <c r="I60">
-        <v>3.388E-3</v>
+        <v>3.571E-3</v>
       </c>
       <c r="J60">
         <v>1</v>
@@ -16516,13 +16519,13 @@
     </row>
     <row r="61" spans="1:11">
       <c r="A61" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B61" t="s">
         <v>9</v>
       </c>
       <c r="C61" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D61" t="s">
         <v>7</v>
@@ -16534,13 +16537,13 @@
         <v>2040</v>
       </c>
       <c r="G61">
-        <v>2015</v>
+        <v>2000</v>
       </c>
       <c r="H61">
-        <v>2015</v>
+        <v>3000</v>
       </c>
       <c r="I61">
-        <v>8.1300000000000001E-3</v>
+        <v>3.388E-3</v>
       </c>
       <c r="J61">
         <v>1</v>
@@ -16551,13 +16554,13 @@
     </row>
     <row r="62" spans="1:11">
       <c r="A62" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B62" t="s">
         <v>9</v>
       </c>
       <c r="C62" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D62" t="s">
         <v>7</v>
@@ -16569,13 +16572,13 @@
         <v>2040</v>
       </c>
       <c r="G62">
-        <v>2800</v>
+        <v>2015</v>
       </c>
       <c r="H62">
-        <v>2800</v>
+        <v>2015</v>
       </c>
       <c r="I62">
-        <v>4.7959999999999999E-3</v>
+        <v>8.1300000000000001E-3</v>
       </c>
       <c r="J62">
         <v>1</v>
@@ -16586,13 +16589,13 @@
     </row>
     <row r="63" spans="1:11">
       <c r="A63" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B63" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C63" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="D63" t="s">
         <v>7</v>
@@ -16604,13 +16607,13 @@
         <v>2040</v>
       </c>
       <c r="G63">
-        <v>600</v>
+        <v>2800</v>
       </c>
       <c r="H63">
-        <v>590</v>
+        <v>2800</v>
       </c>
       <c r="I63">
-        <v>8.4030000000000007E-3</v>
+        <v>4.7959999999999999E-3</v>
       </c>
       <c r="J63">
         <v>1</v>
@@ -16621,13 +16624,13 @@
     </row>
     <row r="64" spans="1:11">
       <c r="A64" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B64" t="s">
         <v>10</v>
       </c>
       <c r="C64" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D64" t="s">
         <v>7</v>
@@ -16639,13 +16642,13 @@
         <v>2040</v>
       </c>
       <c r="G64">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="H64">
-        <v>0</v>
+        <v>590</v>
       </c>
       <c r="I64">
-        <v>4.7959999999999999E-3</v>
+        <v>8.4030000000000007E-3</v>
       </c>
       <c r="J64">
         <v>1</v>
@@ -16656,13 +16659,13 @@
     </row>
     <row r="65" spans="1:11">
       <c r="A65" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B65" t="s">
         <v>10</v>
       </c>
       <c r="C65" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D65" t="s">
         <v>7</v>
@@ -16674,13 +16677,13 @@
         <v>2040</v>
       </c>
       <c r="G65">
-        <v>1700</v>
+        <v>0</v>
       </c>
       <c r="H65">
-        <v>1300</v>
+        <v>0</v>
       </c>
       <c r="I65">
-        <v>5.5469999999999998E-3</v>
+        <v>4.7959999999999999E-3</v>
       </c>
       <c r="J65">
         <v>1</v>
@@ -16691,13 +16694,13 @@
     </row>
     <row r="66" spans="1:11">
       <c r="A66" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B66" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C66" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D66" t="s">
         <v>7</v>
@@ -16709,13 +16712,13 @@
         <v>2040</v>
       </c>
       <c r="G66">
-        <v>700</v>
+        <v>1700</v>
       </c>
       <c r="H66">
-        <v>700</v>
+        <v>1300</v>
       </c>
       <c r="I66">
-        <v>4.7959999999999999E-3</v>
+        <v>5.5469999999999998E-3</v>
       </c>
       <c r="J66">
         <v>1</v>
@@ -16726,13 +16729,13 @@
     </row>
     <row r="67" spans="1:11">
       <c r="A67" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B67" t="s">
         <v>11</v>
       </c>
       <c r="C67" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D67" t="s">
         <v>7</v>
@@ -16744,13 +16747,13 @@
         <v>2040</v>
       </c>
       <c r="G67">
-        <v>1632</v>
+        <v>700</v>
       </c>
       <c r="H67">
-        <v>1632</v>
+        <v>700</v>
       </c>
       <c r="I67">
-        <v>2.3080000000000002E-3</v>
+        <v>4.7959999999999999E-3</v>
       </c>
       <c r="J67">
         <v>1</v>
@@ -16761,13 +16764,13 @@
     </row>
     <row r="68" spans="1:11">
       <c r="A68" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B68" t="s">
         <v>11</v>
       </c>
       <c r="C68" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D68" t="s">
         <v>7</v>
@@ -16779,13 +16782,13 @@
         <v>2040</v>
       </c>
       <c r="G68">
-        <v>715</v>
+        <v>1632</v>
       </c>
       <c r="H68">
-        <v>715</v>
+        <v>1632</v>
       </c>
       <c r="I68">
-        <v>6.8729999999999998E-3</v>
+        <v>2.3080000000000002E-3</v>
       </c>
       <c r="J68">
         <v>1</v>
@@ -16796,13 +16799,13 @@
     </row>
     <row r="69" spans="1:11">
       <c r="A69" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B69" t="s">
         <v>11</v>
       </c>
       <c r="C69" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D69" t="s">
         <v>7</v>
@@ -16814,13 +16817,13 @@
         <v>2040</v>
       </c>
       <c r="G69">
-        <v>2800</v>
+        <v>715</v>
       </c>
       <c r="H69">
-        <v>2800</v>
+        <v>715</v>
       </c>
       <c r="I69">
-        <v>4.7959999999999999E-3</v>
+        <v>6.8729999999999998E-3</v>
       </c>
       <c r="J69">
         <v>1</v>
@@ -16831,13 +16834,13 @@
     </row>
     <row r="70" spans="1:11">
       <c r="A70" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B70" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C70" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="D70" t="s">
         <v>7</v>
@@ -16849,13 +16852,13 @@
         <v>2040</v>
       </c>
       <c r="G70">
-        <v>1716</v>
+        <v>2800</v>
       </c>
       <c r="H70">
-        <v>1716</v>
+        <v>2800</v>
       </c>
       <c r="I70">
-        <v>3.2859999999999999E-3</v>
+        <v>4.7959999999999999E-3</v>
       </c>
       <c r="J70">
         <v>1</v>
@@ -16866,13 +16869,13 @@
     </row>
     <row r="71" spans="1:11">
       <c r="A71" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B71" t="s">
         <v>12</v>
       </c>
       <c r="C71" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D71" t="s">
         <v>7</v>
@@ -16884,13 +16887,13 @@
         <v>2040</v>
       </c>
       <c r="G71">
-        <v>1950</v>
+        <v>1716</v>
       </c>
       <c r="H71">
-        <v>1879</v>
+        <v>1716</v>
       </c>
       <c r="I71">
-        <v>3.3059999999999999E-3</v>
+        <v>3.2859999999999999E-3</v>
       </c>
       <c r="J71">
         <v>1</v>
@@ -16901,13 +16904,13 @@
     </row>
     <row r="72" spans="1:11">
       <c r="A72" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B72" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C72" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D72" t="s">
         <v>7</v>
@@ -16919,13 +16922,13 @@
         <v>2040</v>
       </c>
       <c r="G72">
-        <v>6500</v>
+        <v>1950</v>
       </c>
       <c r="H72">
-        <v>6500</v>
+        <v>1879</v>
       </c>
       <c r="I72">
-        <v>4.627E-3</v>
+        <v>3.3059999999999999E-3</v>
       </c>
       <c r="J72">
         <v>1</v>
@@ -16936,13 +16939,13 @@
     </row>
     <row r="73" spans="1:11">
       <c r="A73" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B73" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C73" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D73" t="s">
         <v>7</v>
@@ -16954,13 +16957,13 @@
         <v>2040</v>
       </c>
       <c r="G73">
-        <v>0</v>
+        <v>6500</v>
       </c>
       <c r="H73">
-        <v>0</v>
+        <v>6500</v>
       </c>
       <c r="I73">
-        <v>4.7959999999999999E-3</v>
+        <v>4.627E-3</v>
       </c>
       <c r="J73">
         <v>1</v>
@@ -16971,13 +16974,13 @@
     </row>
     <row r="74" spans="1:11">
       <c r="A74" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B74" t="s">
         <v>14</v>
       </c>
       <c r="C74" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D74" t="s">
         <v>7</v>
@@ -16989,13 +16992,13 @@
         <v>2040</v>
       </c>
       <c r="G74">
-        <v>2800</v>
+        <v>0</v>
       </c>
       <c r="H74">
-        <v>2800</v>
+        <v>0</v>
       </c>
       <c r="I74">
-        <v>2.9039999999999999E-3</v>
+        <v>4.7959999999999999E-3</v>
       </c>
       <c r="J74">
         <v>1</v>
@@ -17006,13 +17009,13 @@
     </row>
     <row r="75" spans="1:11">
       <c r="A75" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B75" t="s">
         <v>14</v>
       </c>
       <c r="C75" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D75" t="s">
         <v>7</v>
@@ -17024,13 +17027,13 @@
         <v>2040</v>
       </c>
       <c r="G75">
-        <v>1200</v>
+        <v>2800</v>
       </c>
       <c r="H75">
-        <v>1200</v>
+        <v>2800</v>
       </c>
       <c r="I75">
-        <v>4.1539999999999997E-3</v>
+        <v>2.9039999999999999E-3</v>
       </c>
       <c r="J75">
         <v>1</v>
@@ -17041,13 +17044,13 @@
     </row>
     <row r="76" spans="1:11">
       <c r="A76" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B76" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C76" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D76" t="s">
         <v>7</v>
@@ -17059,13 +17062,13 @@
         <v>2040</v>
       </c>
       <c r="G76">
-        <v>8725</v>
+        <v>1200</v>
       </c>
       <c r="H76">
-        <v>8725</v>
+        <v>1200</v>
       </c>
       <c r="I76">
-        <v>4.3889999999999997E-3</v>
+        <v>4.1539999999999997E-3</v>
       </c>
       <c r="J76">
         <v>1</v>
@@ -17076,13 +17079,13 @@
     </row>
     <row r="77" spans="1:11">
       <c r="A77" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B77" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C77" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D77" t="s">
         <v>7</v>
@@ -17094,13 +17097,13 @@
         <v>2040</v>
       </c>
       <c r="G77">
-        <v>950</v>
+        <v>8725</v>
       </c>
       <c r="H77">
-        <v>950</v>
+        <v>8725</v>
       </c>
       <c r="I77">
-        <v>3.3210000000000002E-3</v>
+        <v>4.3889999999999997E-3</v>
       </c>
       <c r="J77">
         <v>1</v>
@@ -17111,13 +17114,13 @@
     </row>
     <row r="78" spans="1:11">
       <c r="A78" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B78" t="s">
         <v>16</v>
       </c>
       <c r="C78" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D78" t="s">
         <v>7</v>
@@ -17129,13 +17132,13 @@
         <v>2040</v>
       </c>
       <c r="G78">
-        <v>700</v>
+        <v>950</v>
       </c>
       <c r="H78">
-        <v>700</v>
+        <v>950</v>
       </c>
       <c r="I78">
-        <v>8.796E-3</v>
+        <v>3.3210000000000002E-3</v>
       </c>
       <c r="J78">
         <v>1</v>
@@ -17146,13 +17149,13 @@
     </row>
     <row r="79" spans="1:11">
       <c r="A79" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B79" t="s">
         <v>16</v>
       </c>
       <c r="C79" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D79" t="s">
         <v>7</v>
@@ -17170,7 +17173,7 @@
         <v>700</v>
       </c>
       <c r="I79">
-        <v>4.8089999999999999E-3</v>
+        <v>8.796E-3</v>
       </c>
       <c r="J79">
         <v>1</v>
@@ -17181,13 +17184,13 @@
     </row>
     <row r="80" spans="1:11">
       <c r="A80" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B80" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C80" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D80" t="s">
         <v>7</v>
@@ -17205,7 +17208,7 @@
         <v>700</v>
       </c>
       <c r="I80">
-        <v>3.813E-3</v>
+        <v>4.8089999999999999E-3</v>
       </c>
       <c r="J80">
         <v>1</v>
@@ -17216,13 +17219,13 @@
     </row>
     <row r="81" spans="1:11">
       <c r="A81" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B81" t="s">
         <v>18</v>
       </c>
       <c r="C81" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D81" t="s">
         <v>7</v>
@@ -17234,13 +17237,13 @@
         <v>2040</v>
       </c>
       <c r="G81">
-        <v>2800</v>
+        <v>700</v>
       </c>
       <c r="H81">
-        <v>2800</v>
+        <v>700</v>
       </c>
       <c r="I81">
-        <v>9.7680000000000006E-3</v>
+        <v>3.813E-3</v>
       </c>
       <c r="J81">
         <v>1</v>
@@ -17251,13 +17254,13 @@
     </row>
     <row r="82" spans="1:11">
       <c r="A82" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B82" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C82" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D82" t="s">
         <v>7</v>
@@ -17269,13 +17272,13 @@
         <v>2040</v>
       </c>
       <c r="G82">
-        <v>350</v>
+        <v>2800</v>
       </c>
       <c r="H82">
-        <v>1300</v>
+        <v>2800</v>
       </c>
       <c r="I82">
-        <v>2.5279999999999999E-3</v>
+        <v>9.7680000000000006E-3</v>
       </c>
       <c r="J82">
         <v>1</v>
@@ -17286,13 +17289,13 @@
     </row>
     <row r="83" spans="1:11">
       <c r="A83" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B83" t="s">
         <v>19</v>
       </c>
       <c r="C83" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D83" t="s">
         <v>7</v>
@@ -17304,13 +17307,13 @@
         <v>2040</v>
       </c>
       <c r="G83">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="H83">
-        <v>600</v>
+        <v>1300</v>
       </c>
       <c r="I83">
-        <v>1.603E-3</v>
+        <v>2.5279999999999999E-3</v>
       </c>
       <c r="J83">
         <v>1</v>
@@ -17321,13 +17324,13 @@
     </row>
     <row r="84" spans="1:11">
       <c r="A84" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B84" t="s">
         <v>19</v>
       </c>
       <c r="C84" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D84" t="s">
         <v>7</v>
@@ -17339,13 +17342,13 @@
         <v>2040</v>
       </c>
       <c r="G84">
+        <v>800</v>
+      </c>
+      <c r="H84">
         <v>600</v>
       </c>
-      <c r="H84">
-        <v>1000</v>
-      </c>
       <c r="I84">
-        <v>3.9880000000000002E-3</v>
+        <v>1.603E-3</v>
       </c>
       <c r="J84">
         <v>1</v>
@@ -17356,13 +17359,13 @@
     </row>
     <row r="85" spans="1:11">
       <c r="A85" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B85" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C85" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D85" t="s">
         <v>7</v>
@@ -17374,13 +17377,13 @@
         <v>2040</v>
       </c>
       <c r="G85">
-        <v>700</v>
+        <v>600</v>
       </c>
       <c r="H85">
-        <v>600</v>
+        <v>1000</v>
       </c>
       <c r="I85">
-        <v>4.3309999999999998E-3</v>
+        <v>3.9880000000000002E-3</v>
       </c>
       <c r="J85">
         <v>1</v>
@@ -17391,13 +17394,13 @@
     </row>
     <row r="86" spans="1:11">
       <c r="A86" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B86" t="s">
         <v>20</v>
       </c>
       <c r="C86" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D86" t="s">
         <v>7</v>
@@ -17409,13 +17412,13 @@
         <v>2040</v>
       </c>
       <c r="G86">
-        <v>250</v>
+        <v>700</v>
       </c>
       <c r="H86">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="I86">
-        <v>3.2550000000000001E-3</v>
+        <v>4.3309999999999998E-3</v>
       </c>
       <c r="J86">
         <v>1</v>
@@ -17426,13 +17429,13 @@
     </row>
     <row r="87" spans="1:11">
       <c r="A87" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B87" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C87" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D87" t="s">
         <v>7</v>
@@ -17444,13 +17447,13 @@
         <v>2040</v>
       </c>
       <c r="G87">
-        <v>2145</v>
+        <v>250</v>
       </c>
       <c r="H87">
-        <v>2095</v>
+        <v>300</v>
       </c>
       <c r="I87">
-        <v>4.248E-3</v>
+        <v>3.2550000000000001E-3</v>
       </c>
       <c r="J87">
         <v>1</v>
@@ -17461,13 +17464,13 @@
     </row>
     <row r="88" spans="1:11">
       <c r="A88" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B88" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C88" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D88" t="s">
         <v>7</v>
@@ -17479,13 +17482,13 @@
         <v>2040</v>
       </c>
       <c r="G88">
-        <v>600</v>
+        <v>2145</v>
       </c>
       <c r="H88">
-        <v>600</v>
+        <v>2095</v>
       </c>
       <c r="I88">
-        <v>8.3330000000000001E-3</v>
+        <v>4.248E-3</v>
       </c>
       <c r="J88">
         <v>1</v>
@@ -17496,13 +17499,13 @@
     </row>
     <row r="89" spans="1:11">
       <c r="A89" t="s">
-        <v>132</v>
+        <v>258</v>
       </c>
       <c r="B89" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C89" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D89" t="s">
         <v>7</v>
@@ -17514,13 +17517,13 @@
         <v>2040</v>
       </c>
       <c r="G89">
-        <v>3300</v>
+        <v>1400</v>
       </c>
       <c r="H89">
-        <v>3300</v>
+        <v>1400</v>
       </c>
       <c r="I89">
-        <v>2.1359999999999999E-3</v>
+        <v>2.7680000000000001E-3</v>
       </c>
       <c r="J89">
         <v>1</v>
@@ -17531,13 +17534,13 @@
     </row>
     <row r="90" spans="1:11">
       <c r="A90" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B90" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C90" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D90" t="s">
         <v>7</v>
@@ -17549,13 +17552,13 @@
         <v>2040</v>
       </c>
       <c r="G90">
-        <v>7300</v>
+        <v>600</v>
       </c>
       <c r="H90">
-        <v>7300</v>
+        <v>600</v>
       </c>
       <c r="I90">
-        <v>1.8680000000000001E-3</v>
+        <v>8.3330000000000001E-3</v>
       </c>
       <c r="J90">
         <v>1</v>
@@ -17566,13 +17569,13 @@
     </row>
     <row r="91" spans="1:11">
       <c r="A91" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B91" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C91" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D91" t="s">
         <v>7</v>
@@ -17584,18 +17587,88 @@
         <v>2040</v>
       </c>
       <c r="G91">
-        <v>6200</v>
+        <v>3300</v>
       </c>
       <c r="H91">
-        <v>2800</v>
+        <v>3300</v>
       </c>
       <c r="I91">
-        <v>2.679E-3</v>
+        <v>2.1359999999999999E-3</v>
       </c>
       <c r="J91">
         <v>1</v>
       </c>
       <c r="K91">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11">
+      <c r="A92" t="s">
+        <v>133</v>
+      </c>
+      <c r="B92" t="s">
+        <v>24</v>
+      </c>
+      <c r="C92" t="s">
+        <v>25</v>
+      </c>
+      <c r="D92" t="s">
+        <v>7</v>
+      </c>
+      <c r="E92" t="s">
+        <v>8</v>
+      </c>
+      <c r="F92">
+        <v>2040</v>
+      </c>
+      <c r="G92">
+        <v>7300</v>
+      </c>
+      <c r="H92">
+        <v>7300</v>
+      </c>
+      <c r="I92">
+        <v>1.8680000000000001E-3</v>
+      </c>
+      <c r="J92">
+        <v>1</v>
+      </c>
+      <c r="K92">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11">
+      <c r="A93" t="s">
+        <v>134</v>
+      </c>
+      <c r="B93" t="s">
+        <v>25</v>
+      </c>
+      <c r="C93" t="s">
+        <v>26</v>
+      </c>
+      <c r="D93" t="s">
+        <v>7</v>
+      </c>
+      <c r="E93" t="s">
+        <v>8</v>
+      </c>
+      <c r="F93">
+        <v>2040</v>
+      </c>
+      <c r="G93">
+        <v>6200</v>
+      </c>
+      <c r="H93">
+        <v>2800</v>
+      </c>
+      <c r="I93">
+        <v>2.679E-3</v>
+      </c>
+      <c r="J93">
+        <v>1</v>
+      </c>
+      <c r="K93">
         <v>0.01</v>
       </c>
     </row>
@@ -17614,8 +17687,8 @@
   </sheetPr>
   <dimension ref="A1:AO3"/>
   <sheetViews>
-    <sheetView topLeftCell="AD1" workbookViewId="0">
-      <selection activeCell="AG1" sqref="AG1:AG1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17946,7 +18019,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18422,7 +18495,7 @@
   </sheetPr>
   <dimension ref="A1:L93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Adding an option for 'all' to country column. Adding country level fuel data.
</commit_message>
<xml_diff>
--- a/src_files/data_files/TYNDP-2024_National_Trends.xlsx
+++ b/src_files/data_files/TYNDP-2024_National_Trends.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BB\bb-master\north_european_model\src_files\data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C778B319-F1D1-4C03-B442-2E14D1A73627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD589B83-82E9-4843-B962-E92BCFB4F0A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="862" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="862" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="9" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3242" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3263" uniqueCount="215">
   <si>
     <t>Country</t>
   </si>
@@ -1242,7 +1242,29 @@
     <cellStyle name="Normal 5" xfId="2" xr:uid="{3F0C574D-7EC4-4897-89EC-E327150F272B}"/>
     <cellStyle name="Standard_Data provided by OT3" xfId="6" xr:uid="{1E95AE55-13E4-4211-A613-AFC1DB5E5A34}"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="18">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
     <dxf>
       <border outline="0">
         <top style="thin">
@@ -1290,25 +1312,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -1499,7 +1502,7 @@
       <sheetName val="data_fuelEmissions"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
+      <sheetData sheetId="0" refreshError="1"/>
       <sheetData sheetId="1">
         <row r="4">
           <cell r="E4" t="str">
@@ -1623,7 +1626,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{4481F0AF-41D8-47A8-8506-AC52CB6AB7F9}" name="Table5" displayName="Table5" ref="A1:H616" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{4481F0AF-41D8-47A8-8506-AC52CB6AB7F9}" name="Table5" displayName="Table5" ref="A1:H616" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12">
   <autoFilter ref="A1:H616" xr:uid="{4481F0AF-41D8-47A8-8506-AC52CB6AB7F9}">
     <filterColumn colId="1">
       <filters>
@@ -1647,7 +1650,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BE65DD6F-AEBC-42F9-B7B9-FF669064D0A0}" name="Table4" displayName="Table4" ref="A1:G45" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BE65DD6F-AEBC-42F9-B7B9-FF669064D0A0}" name="Table4" displayName="Table4" ref="A1:G45" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9">
   <autoFilter ref="A1:G45" xr:uid="{BE65DD6F-AEBC-42F9-B7B9-FF669064D0A0}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{4DDF1ABC-FF46-4BB6-A809-F638501F6746}" name="Country"/>
@@ -1663,7 +1666,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{B440C99F-3BB1-4A8C-9867-FC60A58307DE}" name="Table6" displayName="Table6" ref="A1:I1048576" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="15" tableBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{B440C99F-3BB1-4A8C-9867-FC60A58307DE}" name="Table6" displayName="Table6" ref="A1:I1048576" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15">
   <autoFilter ref="A1:I1048576" xr:uid="{B440C99F-3BB1-4A8C-9867-FC60A58307DE}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{02926FC6-CA21-44BB-975F-A929C6C412D4}" name="grid"/>
@@ -1681,15 +1684,16 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D9844F2F-2EE0-434B-9492-0280A28AB057}" name="Table8" displayName="Table8" ref="A1:E21" totalsRowShown="0" headerRowDxfId="7">
-  <autoFilter ref="A1:E21" xr:uid="{D9844F2F-2EE0-434B-9492-0280A28AB057}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{EE76C5C2-E9D6-4CA0-9ABF-B1C7F3426312}" name="Scenario" dataDxfId="6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D9844F2F-2EE0-434B-9492-0280A28AB057}" name="Table8" displayName="Table8" ref="A1:F21" totalsRowShown="0" headerRowDxfId="8">
+  <autoFilter ref="A1:F21" xr:uid="{D9844F2F-2EE0-434B-9492-0280A28AB057}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{EE76C5C2-E9D6-4CA0-9ABF-B1C7F3426312}" name="Scenario" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{40AE79E8-AB14-466F-AE4B-226B9D11277C}" name="Year"/>
-    <tableColumn id="3" xr3:uid="{9172289D-E869-498C-9DCD-9CEC866DBBD2}" name="grid" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{AEC998FA-121F-4D1C-B1B1-FC7C7DDBA7AE}" name="price" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{9056A538-46B6-4FAC-AA92-94F33B818677}" name="emission_CO2" dataDxfId="3">
-      <calculatedColumnFormula>IFERROR(VLOOKUP($C2, [1]data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</calculatedColumnFormula>
+    <tableColumn id="6" xr3:uid="{F58D1D29-CB7C-4B03-8AC3-0955B77DC71F}" name="Country" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{9172289D-E869-498C-9DCD-9CEC866DBBD2}" name="grid" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{AEC998FA-121F-4D1C-B1B1-FC7C7DDBA7AE}" name="price" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{9056A538-46B6-4FAC-AA92-94F33B818677}" name="emission_CO2" dataDxfId="5">
+      <calculatedColumnFormula>IFERROR(VLOOKUP($D2, [1]data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1697,7 +1701,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{9719B7EE-3FF9-4612-B637-C2081C2392C1}" name="Table7" displayName="Table7" ref="A1:L93" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{9719B7EE-3FF9-4612-B637-C2081C2392C1}" name="Table7" displayName="Table7" ref="A1:L93" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2">
   <autoFilter ref="A1:L93" xr:uid="{9719B7EE-3FF9-4612-B637-C2081C2392C1}">
     <filterColumn colId="2">
       <filters>
@@ -14288,7 +14292,7 @@
   </sheetPr>
   <dimension ref="A1:I185"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
@@ -20085,395 +20089,459 @@
   <sheetPr>
     <tabColor theme="6" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="33" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="28" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="E1" s="29" t="s">
         <v>161</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="F1" s="29" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" s="30" t="s">
         <v>8</v>
       </c>
       <c r="B2">
         <v>2030</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="D2" s="31" t="s">
         <v>163</v>
       </c>
-      <c r="D2" s="32">
+      <c r="E2" s="32">
         <v>27</v>
       </c>
-      <c r="E2" s="33">
-        <f>IFERROR(VLOOKUP($C2, [1]data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+      <c r="F2" s="33">
+        <f>IFERROR(VLOOKUP($D2, [1]data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
         <v>0.34200000000000003</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3" s="30" t="s">
         <v>8</v>
       </c>
       <c r="B3">
         <v>2030</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="D3" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="32">
+      <c r="E3" s="32">
         <v>2.5</v>
       </c>
-      <c r="E3" s="33">
-        <f>IFERROR(VLOOKUP($C3, [1]data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+      <c r="F3" s="33">
+        <f>IFERROR(VLOOKUP($D3, [1]data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4" s="30" t="s">
         <v>8</v>
       </c>
       <c r="B4">
         <v>2030</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="D4" s="31" t="s">
         <v>164</v>
       </c>
-      <c r="D4" s="32">
+      <c r="E4" s="32">
         <v>55</v>
       </c>
-      <c r="E4" s="33">
-        <f>IFERROR(VLOOKUP($C4, [1]data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+      <c r="F4" s="33">
+        <f>IFERROR(VLOOKUP($D4, [1]data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
         <v>0.19800000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5" s="30" t="s">
         <v>8</v>
       </c>
       <c r="B5">
         <v>2030</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="D5" s="31" t="s">
         <v>165</v>
       </c>
-      <c r="D5" s="32">
+      <c r="E5" s="32">
         <v>46</v>
       </c>
-      <c r="E5" s="33">
-        <f>IFERROR(VLOOKUP($C5, [1]data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+      <c r="F5" s="33">
+        <f>IFERROR(VLOOKUP($D5, [1]data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
         <v>0.28079999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6">
       <c r="A6" s="30" t="s">
         <v>8</v>
       </c>
       <c r="B6">
         <v>2030</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="D6" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="32">
+      <c r="E6" s="32">
         <v>65</v>
       </c>
-      <c r="E6" s="33">
-        <f>IFERROR(VLOOKUP($C6, [1]data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+      <c r="F6" s="33">
+        <f>IFERROR(VLOOKUP($D6, [1]data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
         <v>0.25559999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:6">
       <c r="A7" s="30" t="s">
         <v>8</v>
       </c>
       <c r="B7">
         <v>2030</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="D7" s="31" t="s">
         <v>166</v>
       </c>
-      <c r="D7" s="34">
-        <v>8</v>
-      </c>
-      <c r="E7" s="33">
-        <f>IFERROR(VLOOKUP($C7, [1]data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+      <c r="E7" s="34">
+        <v>8</v>
+      </c>
+      <c r="F7" s="33">
+        <f>IFERROR(VLOOKUP($D7, [1]data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
         <v>0.37080000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:6">
       <c r="A8" s="30" t="s">
         <v>8</v>
       </c>
       <c r="B8">
         <v>2030</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="D8" s="31" t="s">
         <v>167</v>
       </c>
-      <c r="D8" s="32">
+      <c r="E8" s="32">
         <v>26</v>
       </c>
-      <c r="E8" s="33">
-        <f>IFERROR(VLOOKUP($C8, [1]data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+      <c r="F8" s="33">
+        <f>IFERROR(VLOOKUP($D8, [1]data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:6">
       <c r="A9" s="30" t="s">
         <v>8</v>
       </c>
       <c r="B9">
         <v>2030</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="D9" s="31" t="s">
         <v>168</v>
       </c>
-      <c r="D9" s="33">
+      <c r="E9" s="33">
         <v>1</v>
       </c>
-      <c r="E9" s="33">
-        <f>IFERROR(VLOOKUP($C9, [1]data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+      <c r="F9" s="33">
+        <f>IFERROR(VLOOKUP($D9, [1]data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:6">
       <c r="A10" s="30" t="s">
         <v>8</v>
       </c>
       <c r="B10">
         <v>2030</v>
       </c>
-      <c r="C10" s="31" t="s">
+      <c r="C10" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="D10" s="31" t="s">
         <v>169</v>
       </c>
-      <c r="D10" s="33">
+      <c r="E10" s="33">
         <v>1</v>
       </c>
-      <c r="E10" s="33">
-        <f>IFERROR(VLOOKUP($C10, [1]data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+      <c r="F10" s="33">
+        <f>IFERROR(VLOOKUP($D10, [1]data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
         <v>0.14399999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:6">
       <c r="A11" s="30" t="s">
         <v>8</v>
       </c>
       <c r="B11">
         <v>2030</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="D11" t="s">
         <v>170</v>
       </c>
-      <c r="D11" s="33">
+      <c r="E11" s="33">
         <v>10</v>
       </c>
-      <c r="E11" s="33">
-        <f>IFERROR(VLOOKUP($C11, [1]data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+      <c r="F11" s="33">
+        <f>IFERROR(VLOOKUP($D11, [1]data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
         <v>0.41399999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:6">
       <c r="A12" s="30" t="s">
         <v>8</v>
       </c>
       <c r="B12">
         <v>2040</v>
       </c>
-      <c r="C12" s="31" t="s">
+      <c r="C12" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="D12" s="31" t="s">
         <v>163</v>
       </c>
-      <c r="D12" s="32">
+      <c r="E12" s="32">
         <v>27</v>
       </c>
-      <c r="E12" s="33">
-        <f>IFERROR(VLOOKUP($C12, [1]data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+      <c r="F12" s="33">
+        <f>IFERROR(VLOOKUP($D12, [1]data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
         <v>0.34200000000000003</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:6">
       <c r="A13" s="30" t="s">
         <v>8</v>
       </c>
       <c r="B13">
         <v>2040</v>
       </c>
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="D13" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="32">
+      <c r="E13" s="32">
         <v>2.5</v>
       </c>
-      <c r="E13" s="33">
-        <f>IFERROR(VLOOKUP($C13, [1]data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+      <c r="F13" s="33">
+        <f>IFERROR(VLOOKUP($D13, [1]data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:6">
       <c r="A14" s="30" t="s">
         <v>8</v>
       </c>
       <c r="B14">
         <v>2040</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="D14" s="31" t="s">
         <v>164</v>
       </c>
-      <c r="D14" s="32">
+      <c r="E14" s="32">
         <v>55</v>
       </c>
-      <c r="E14" s="33">
-        <f>IFERROR(VLOOKUP($C14, [1]data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+      <c r="F14" s="33">
+        <f>IFERROR(VLOOKUP($D14, [1]data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
         <v>0.19800000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:6">
       <c r="A15" s="30" t="s">
         <v>8</v>
       </c>
       <c r="B15">
         <v>2040</v>
       </c>
-      <c r="C15" s="31" t="s">
+      <c r="C15" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="D15" s="31" t="s">
         <v>165</v>
       </c>
-      <c r="D15" s="32">
+      <c r="E15" s="32">
         <v>46</v>
       </c>
-      <c r="E15" s="33">
-        <f>IFERROR(VLOOKUP($C15, [1]data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+      <c r="F15" s="33">
+        <f>IFERROR(VLOOKUP($D15, [1]data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
         <v>0.28079999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:6">
       <c r="A16" s="30" t="s">
         <v>8</v>
       </c>
       <c r="B16">
         <v>2040</v>
       </c>
-      <c r="C16" s="31" t="s">
+      <c r="C16" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="D16" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="D16" s="32">
+      <c r="E16" s="32">
         <v>65</v>
       </c>
-      <c r="E16" s="33">
-        <f>IFERROR(VLOOKUP($C16, [1]data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+      <c r="F16" s="33">
+        <f>IFERROR(VLOOKUP($D16, [1]data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
         <v>0.25559999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:6">
       <c r="A17" s="30" t="s">
         <v>8</v>
       </c>
       <c r="B17">
         <v>2040</v>
       </c>
-      <c r="C17" s="31" t="s">
+      <c r="C17" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="D17" s="31" t="s">
         <v>166</v>
       </c>
-      <c r="D17" s="34">
-        <v>8</v>
-      </c>
-      <c r="E17" s="33">
-        <f>IFERROR(VLOOKUP($C17, [1]data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+      <c r="E17" s="34">
+        <v>8</v>
+      </c>
+      <c r="F17" s="33">
+        <f>IFERROR(VLOOKUP($D17, [1]data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
         <v>0.37080000000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:6">
       <c r="A18" s="30" t="s">
         <v>8</v>
       </c>
       <c r="B18">
         <v>2040</v>
       </c>
-      <c r="C18" s="31" t="s">
+      <c r="C18" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="D18" s="31" t="s">
         <v>167</v>
       </c>
-      <c r="D18" s="32">
+      <c r="E18" s="32">
         <v>26</v>
       </c>
-      <c r="E18" s="33">
-        <f>IFERROR(VLOOKUP($C18, [1]data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+      <c r="F18" s="33">
+        <f>IFERROR(VLOOKUP($D18, [1]data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:6">
       <c r="A19" s="30" t="s">
         <v>8</v>
       </c>
       <c r="B19">
         <v>2040</v>
       </c>
-      <c r="C19" s="31" t="s">
+      <c r="C19" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="D19" s="31" t="s">
         <v>168</v>
       </c>
-      <c r="D19" s="33">
+      <c r="E19" s="33">
         <v>1</v>
       </c>
-      <c r="E19" s="33">
-        <f>IFERROR(VLOOKUP($C19, [1]data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+      <c r="F19" s="33">
+        <f>IFERROR(VLOOKUP($D19, [1]data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:6">
       <c r="A20" s="30" t="s">
         <v>8</v>
       </c>
       <c r="B20">
         <v>2040</v>
       </c>
-      <c r="C20" s="31" t="s">
+      <c r="C20" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="D20" s="31" t="s">
         <v>169</v>
       </c>
-      <c r="D20" s="33">
+      <c r="E20" s="33">
         <v>1</v>
       </c>
-      <c r="E20" s="33">
-        <f>IFERROR(VLOOKUP($C20, [1]data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+      <c r="F20" s="33">
+        <f>IFERROR(VLOOKUP($D20, [1]data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
         <v>0.14399999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:6">
       <c r="A21" s="30" t="s">
         <v>8</v>
       </c>
       <c r="B21">
         <v>2040</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="D21" t="s">
         <v>170</v>
       </c>
-      <c r="D21" s="33">
+      <c r="E21" s="33">
         <v>10</v>
       </c>
-      <c r="E21" s="33">
-        <f>IFERROR(VLOOKUP($C21, [1]data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+      <c r="F21" s="33">
+        <f>IFERROR(VLOOKUP($D21, [1]data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
         <v>0.41399999999999998</v>
       </c>
     </row>

</xml_diff>